<commit_message>
Clear Prev Printing Queue Before Resending
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Codebar_Benki\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SorazaImport\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECCC89E-4B77-47B2-8221-CD81CFD1E544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1F0C9D-AF4B-4EF9-9E7B-333363B3D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SX010-AFA</t>
-  </si>
-  <si>
-    <t>SX010</t>
+    <t>SD008-Ajicero</t>
+  </si>
+  <si>
+    <t>SD008</t>
   </si>
 </sst>
 </file>
@@ -164,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -310,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>10</v>

</xml_diff>

<commit_message>
Include a Recovery on Non Closed Session
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SorazaImport\Desktop\codebarPrintingTool\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1F0C9D-AF4B-4EF9-9E7B-333363B3D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA44EA8-12AF-434D-9E9E-877030C109C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SD008-Ajicero</t>
-  </si>
-  <si>
-    <t>SD008</t>
+    <t>F030-PANTALONETA</t>
+  </si>
+  <si>
+    <t>F030</t>
   </si>
 </sst>
 </file>
@@ -164,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -310,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="H2">
         <v>10</v>

</xml_diff>

<commit_message>
fix saved on closed
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA44EA8-12AF-434D-9E9E-877030C109C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0116697B-505B-4CF5-81BC-E9F4B54D27C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,7 +467,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>

</xml_diff>

<commit_message>
Zoom, Val, Default New Item Name, clear Verification
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\codebarPrintingTool\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0116697B-505B-4CF5-81BC-E9F4B54D27C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D3F3B-2A03-42C7-A2D7-AD83789B4BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>F030-PANTALONETA</t>
-  </si>
-  <si>
-    <t>F030</t>
+    <t>SQ009-DELINEADOR</t>
+  </si>
+  <si>
+    <t>SQ009</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,7 +467,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="H2">
         <v>10</v>

</xml_diff>

<commit_message>
Almacen Button Selector - FIX
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D3F3B-2A03-42C7-A2D7-AD83789B4BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B976B5C8-F874-45E0-A465-DDBD236993F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="2805" windowWidth="27930" windowHeight="15855" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SQ009-DELINEADOR</t>
-  </si>
-  <si>
     <t>SQ009</t>
+  </si>
+  <si>
+    <t>SQ009-Pulsera</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +549,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -579,10 +579,10 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
         <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Show session items button + bug fixes
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B976B5C8-F874-45E0-A465-DDBD236993F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B491692B-D770-4843-880B-982BECA341EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="2805" windowWidth="27930" windowHeight="15855" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -105,10 +105,34 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SQ009</t>
-  </si>
-  <si>
-    <t>SQ009-Pulsera</t>
+    <t>SP001-Polera</t>
+  </si>
+  <si>
+    <t>SS016-Plancha</t>
+  </si>
+  <si>
+    <t>SZ006-ZAPATERA</t>
+  </si>
+  <si>
+    <t>SA042-RIZADOR</t>
+  </si>
+  <si>
+    <t>SG015-ZAPATO</t>
+  </si>
+  <si>
+    <t>SP001</t>
+  </si>
+  <si>
+    <t>SS016</t>
+  </si>
+  <si>
+    <t>SZ006</t>
+  </si>
+  <si>
+    <t>SA042</t>
+  </si>
+  <si>
+    <t>SG015</t>
   </si>
 </sst>
 </file>
@@ -461,7 +485,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -549,10 +573,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -561,7 +585,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -579,10 +603,162 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="T2" t="s">
-        <v>23</v>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor adjustments printer orientation portrait + language excel selector
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\codebarprintingtool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B491692B-D770-4843-880B-982BECA341EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Nombre</t>
   </si>
@@ -105,40 +104,22 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SP001-Polera</t>
-  </si>
-  <si>
-    <t>SS016-Plancha</t>
-  </si>
-  <si>
-    <t>SZ006-ZAPATERA</t>
-  </si>
-  <si>
-    <t>SA042-RIZADOR</t>
-  </si>
-  <si>
-    <t>SG015-ZAPATO</t>
-  </si>
-  <si>
-    <t>SP001</t>
-  </si>
-  <si>
-    <t>SS016</t>
-  </si>
-  <si>
-    <t>SZ006</t>
-  </si>
-  <si>
-    <t>SA042</t>
-  </si>
-  <si>
-    <t>SG015</t>
+    <t>SR012-Humificador</t>
+  </si>
+  <si>
+    <t>SB034-Porta</t>
+  </si>
+  <si>
+    <t>SR012</t>
+  </si>
+  <si>
+    <t>SB034</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,33 +464,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="38.28515625" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="38.33203125" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,12 +552,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -585,7 +566,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -606,15 +587,15 @@
         <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -623,7 +604,7 @@
         <v>21</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -644,121 +625,7 @@
         <v>24</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
-        <v>80</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pdf genereation version low quality problems
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -104,16 +104,16 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SR012-Humificador</t>
-  </si>
-  <si>
-    <t>SB034-Porta</t>
-  </si>
-  <si>
-    <t>SR012</t>
-  </si>
-  <si>
-    <t>SB034</t>
+    <t>WR005-Plastilina</t>
+  </si>
+  <si>
+    <t>WX001-Juguete</t>
+  </si>
+  <si>
+    <t>WR005</t>
+  </si>
+  <si>
+    <t>WX001</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
         <v>21</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="H3">
         <v>10</v>

</xml_diff>

<commit_message>
just some delete new item fix
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\codebarprintingtool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\barcodeUtils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -104,16 +104,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>WR005-Plastilina</t>
-  </si>
-  <si>
-    <t>WX001-Juguete</t>
-  </si>
-  <si>
-    <t>WR005</t>
-  </si>
-  <si>
-    <t>WX001</t>
+    <t>ST012-Asd</t>
+  </si>
+  <si>
+    <t>ST012</t>
   </si>
 </sst>
 </file>
@@ -466,7 +460,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -557,7 +551,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -566,7 +560,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -587,45 +581,7 @@
         <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>9.5</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix fonts also added prebuild js for production
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\barcodeUtils\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\barcodeUtils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB797F9C-785E-4CF5-8911-D131AF2C0886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -104,16 +105,16 @@
     <t>SI</t>
   </si>
   <si>
-    <t>ST012-Asd</t>
-  </si>
-  <si>
-    <t>ST012</t>
+    <t>WE002-RELOJ</t>
+  </si>
+  <si>
+    <t>WE002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -466,25 +467,25 @@
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="38.33203125" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -560,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>10</v>

</xml_diff>